<commit_message>
Finished with question bank section
</commit_message>
<xml_diff>
--- a/project/templates/tests/faculty/question_template.xlsx
+++ b/project/templates/tests/faculty/question_template.xlsx
@@ -473,7 +473,10 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
+    <dataValidation sqref="G2:G100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>"option 1,option 2,option 3,option 4"</formula1>
+    </dataValidation>
     <dataValidation sqref="G2:G100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"option 1,option 2,option 3,option 4"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Fixing test take bug
</commit_message>
<xml_diff>
--- a/project/templates/tests/faculty/question_template.xlsx
+++ b/project/templates/tests/faculty/question_template.xlsx
@@ -473,7 +473,10 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="6">
+    <dataValidation sqref="G2:G100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>"option 1,option 2,option 3,option 4"</formula1>
+    </dataValidation>
     <dataValidation sqref="G2:G100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"option 1,option 2,option 3,option 4"</formula1>
     </dataValidation>
@@ -534,14 +537,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Chemical Bonding</t>
+          <t>Algebra</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Organic Chemistry</t>
+          <t>Arithmetic</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Migrated to MYSQL and updated to the latest django version
</commit_message>
<xml_diff>
--- a/project/templates/tests/faculty/question_template.xlsx
+++ b/project/templates/tests/faculty/question_template.xlsx
@@ -473,7 +473,22 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataValidations count="11">
+    <dataValidation sqref="G2:G100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>"option 1,option 2,option 3,option 4"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>"option 1,option 2,option 3,option 4"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>"option 1,option 2,option 3,option 4"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>"option 1,option 2,option 3,option 4"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>"option 1,option 2,option 3,option 4"</formula1>
+    </dataValidation>
     <dataValidation sqref="G2:G100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"option 1,option 2,option 3,option 4"</formula1>
     </dataValidation>
@@ -487,7 +502,7 @@
       <formula1>"option 1,option 2,option 3,option 4"</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>'topics'!$A$2:$A$3</formula1>
+      <formula1>'topics'!$A$2:$A$4</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"option 1,option 2,option 3,option 4"</formula1>
@@ -504,7 +519,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,14 +552,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Algebra</t>
+          <t>Inorganic Chemistry</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Arithmetic</t>
+          <t>Thermodynamics</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Organic Chemistry</t>
         </is>
       </c>
     </row>

</xml_diff>